<commit_message>
Creation ressources conformite (#6)
* commit intial

* Delete EclaireResearchStudy-exemple.fsh

* profiling researchstudy

* correction sushi config

* correction sushi config

* Update ECLAIREResearchStudy.fsh

correction typo dans le profil researchStudy

* repare slicing ECLAIREResearchStudy.fsh

---------

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com> 7712c04b2e461f108c206fe789049f4b5c61b6a6
</commit_message>
<xml_diff>
--- a/ig/main/all-profiles.xlsx
+++ b/ig/main/all-profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="322">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-30T10:27:30+00:00</t>
+    <t>2023-06-30T12:07:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -351,7 +351,7 @@
 </t>
   </si>
   <si>
-    <t>Identifiant de l'essai clinique</t>
+    <t>Business Identifier for study</t>
   </si>
   <si>
     <t>Identifiers assigned to this research study by the sponsor or other systems.</t>
@@ -360,14 +360,258 @@
     <t>Allows identification of the research study as it is known by various participating systems and in a way that remains consistent across servers.</t>
   </si>
   <si>
-    <t>ResearchStudy.title</t>
+    <t xml:space="preserve">value:use}
+</t>
+  </si>
+  <si>
+    <t>Slicing pour les différents identifiants de l'essai clinique</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire</t>
+  </si>
+  <si>
+    <t>idPrimaire</t>
+  </si>
+  <si>
+    <t>Identifiant primaire de l'essai clinique / Primary Registry and Trial Identifying Number</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.id</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.id</t>
   </si>
   <si>
     <t xml:space="preserve">string
 </t>
   </si>
   <si>
-    <t>Name for this study</t>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.use</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.use</t>
+  </si>
+  <si>
+    <t>usual | official | temp | secondary | old (If known)</t>
+  </si>
+  <si>
+    <t>The purpose of this identifier.</t>
+  </si>
+  <si>
+    <t>Applications can assume that an identifier is permanent unless it explicitly says that it is temporary.</t>
+  </si>
+  <si>
+    <t>Allows the appropriate identifier for a particular context of use to be selected from among a set of identifiers.</t>
+  </si>
+  <si>
+    <t>usual</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Identifies the purpose for this identifier, if known .</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/identifier-use|4.0.1</t>
+  </si>
+  <si>
+    <t>Identifier.use</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.type</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodeableConcept
+</t>
+  </si>
+  <si>
+    <t>Description of identifier</t>
+  </si>
+  <si>
+    <t>A coded type for the identifier that can be used to determine which identifier to use for a specific purpose.</t>
+  </si>
+  <si>
+    <t>This element deals only with general categories of identifiers.  It SHOULD not be used for codes that correspond 1..1 with the Identifier.system. Some identifiers may fall into multiple categories due to common usage.   Where the system is known, a type is unnecessary because the type is always part of the system definition. However systems often need to handle identifiers where the system is not known. There is not a 1:1 relationship between type and system, since many different systems have the same type.</t>
+  </si>
+  <si>
+    <t>Allows users to make use of identifiers when the identifier system is not known.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+  </si>
+  <si>
+    <t>Identifier.type</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.system</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.system</t>
+  </si>
+  <si>
+    <t>The namespace for the identifier value</t>
+  </si>
+  <si>
+    <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
+  </si>
+  <si>
+    <t>Identifier.system is always case sensitive.</t>
+  </si>
+  <si>
+    <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
+  </si>
+  <si>
+    <t>http://www.acme.com/identifiers/patient</t>
+  </si>
+  <si>
+    <t>Identifier.system</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.value</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.value</t>
+  </si>
+  <si>
+    <t>The value that is unique</t>
+  </si>
+  <si>
+    <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
+  </si>
+  <si>
+    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://hl7.org/fhir/R4/extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Identifier.value</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.period</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period
+</t>
+  </si>
+  <si>
+    <t>Time period when id is/was valid for use</t>
+  </si>
+  <si>
+    <t>Time period during which identifier is/was valid for use.</t>
+  </si>
+  <si>
+    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
+Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
+  </si>
+  <si>
+    <t>Identifier.period</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idPrimaire.assigner</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier.assigner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Organization)
+</t>
+  </si>
+  <si>
+    <t>Organization that issued id (may be just text)</t>
+  </si>
+  <si>
+    <t>Organization that issued/manages the identifier.</t>
+  </si>
+  <si>
+    <t>The Identifier.assigner may omit the .reference element and only contain a .display element reflecting the name or other textual information about the assigning organization.</t>
+  </si>
+  <si>
+    <t>Identifier.assigner</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ref-1:SHALL have a contained resource if a local reference is provided {reference.startsWith('#').not() or (reference.substring(1).trace('url') in %rootResource.contained.id.trace('ids'))}</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire</t>
+  </si>
+  <si>
+    <t>idSecondaire</t>
+  </si>
+  <si>
+    <t>identifiants secondaires / Secondary Identifying Numbers (e.g., protocol number) if available.  Also include other trial registries that have issued an identifying number to this trial. There is no limit on the number of Secondary identifying numbers that can be provided.</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.id</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.use</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.type</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.system</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.value</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.period</t>
+  </si>
+  <si>
+    <t>ResearchStudy.identifier:idSecondaire.assigner</t>
+  </si>
+  <si>
+    <t>ResearchStudy.title</t>
+  </si>
+  <si>
+    <t>Nom de l'étude / Public Title</t>
   </si>
   <si>
     <t>A short, descriptive user-friendly label for the study.</t>
@@ -392,10 +636,6 @@
     <t>References SHALL be a reference to an actual FHIR resource, and SHALL be resolveable (allowing for access control, temporary unavailability, etc.). Resolution can be either by retrieval from the URL, or, where applicable by resource type, by treating an absolute reference as a canonical URL and looking it up in a local registry/repository.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ref-1:SHALL have a contained resource if a local reference is provided {reference.startsWith('#').not() or (reference.substring(1).trace('url') in %rootResource.contained.id.trace('ids'))}</t>
-  </si>
-  <si>
     <t>ResearchStudy.partOf</t>
   </si>
   <si>
@@ -419,15 +659,12 @@
     <t>ResearchStudy.status</t>
   </si>
   <si>
-    <t>active | administratively-completed | approved | closed-to-accrual | closed-to-accrual-and-intervention | completed | disapproved | in-review | temporarily-closed-to-accrual | temporarily-closed-to-accrual-and-intervention | withdrawn</t>
+    <t>Statut du recrutement / Recruitment Status</t>
   </si>
   <si>
     <t>The current state of the study.</t>
   </si>
   <si>
-    <t>required</t>
-  </si>
-  <si>
     <t>Codes that convey the current status of the research study.</t>
   </si>
   <si>
@@ -437,10 +674,6 @@
     <t>ResearchStudy.primaryPurposeType</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept
-</t>
-  </si>
-  <si>
     <t>treatment | prevention | diagnostic | supportive-care | screening | health-services-research | basic-science | device-feasibility</t>
   </si>
   <si>
@@ -450,9 +683,6 @@
     <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
     <t>Codes for the main intent of the study.</t>
   </si>
   <si>
@@ -504,7 +734,7 @@
     <t>ResearchStudy.condition</t>
   </si>
   <si>
-    <t>Condition being studied</t>
+    <t>Sujet concerné /  Problem(s) Studied</t>
   </si>
   <si>
     <t>The condition that is the focus of the study.  For example, In a study to examine risk factors for Lupus, might have as an inclusion criterion "healthy volunteer", but the target condition code would be a Lupus SNOMED code.</t>
@@ -579,7 +809,7 @@
 </t>
   </si>
   <si>
-    <t>What this is study doing</t>
+    <t>Résumé de l'essai / Summary Results</t>
   </si>
   <si>
     <t>A full description of how the study is being conducted.</t>
@@ -599,7 +829,7 @@
 </t>
   </si>
   <si>
-    <t>Inclusion &amp; exclusion criteria</t>
+    <t>Critères d'inclusion et d'exclusion / Inclusion &amp; exclusion criteria</t>
   </si>
   <si>
     <t>Reference to a Group that defines the criteria for and quantity of subjects participating in the study.  E.g. " 200 female Europeans between the ages of 20 and 45 with early onset diabetes".</t>
@@ -615,32 +845,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Period
-</t>
-  </si>
-  <si>
     <t>When the study began and ended</t>
   </si>
   <si>
     <t>Identifies the start date and the expected (or actual, depending on status) end date for the study.</t>
   </si>
   <si>
-    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
-Period is not used for a duration (a measure of elapsed time). See [Duration](http://hl7.org/fhir/R4/datatypes.html#Duration).</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-per-1:If present, start SHALL have a lower value than end {start.hasValue().not() or end.hasValue().not() or (start &lt;= end)}</t>
-  </si>
-  <si>
     <t>ResearchStudy.sponsor</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
-</t>
-  </si>
-  <si>
-    <t>Organization that initiates and is legally responsible for the study</t>
+    <t>promoteur / primary Sponsor</t>
   </si>
   <si>
     <t>An organization that initiates the investigation and is legally responsible for the study.</t>
@@ -719,22 +933,7 @@
     <t>ResearchStudy.arm.id</t>
   </si>
   <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
     <t>ResearchStudy.arm.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>ResearchStudy.arm.modifierExtension</t>
@@ -1123,7 +1322,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK44"/>
+  <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1133,8 +1332,9 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="20.9609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="41.0234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="45.78515625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="41.0234375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="12.98046875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="39.9140625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="2.2109375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="2.2109375" customWidth="true" bestFit="true"/>
@@ -1148,8 +1348,8 @@
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="10.54296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="38.2265625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="1.04296875" customWidth="true" bestFit="true"/>
@@ -1157,13 +1357,12 @@
     <col min="26" max="26" width="124.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="54.97265625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="10.26171875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="42.03515625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="11.08203125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="52.18359375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="1.04296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="5.62109375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="34.859375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="2.2109375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" hidden="true" width="8.0" customWidth="false"/>
     <col min="18" max="18" width="20.703125" customWidth="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
   </cols>
@@ -2129,10 +2328,10 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" t="s" s="2">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>39</v>
@@ -2191,16 +2390,16 @@
         <v>39</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="AE10" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>104</v>
@@ -2223,12 +2422,14 @@
         <v>3</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>112</v>
+      </c>
       <c r="E11" t="s" s="2">
         <v>39</v>
       </c>
@@ -2249,18 +2450,18 @@
         <v>46</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="O11" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="P11" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="Q11" t="s" s="2">
         <v>39</v>
       </c>
@@ -2308,13 +2509,13 @@
         <v>39</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AH11" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>57</v>
@@ -2331,7 +2532,7 @@
         <v>114</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2342,7 +2543,7 @@
         <v>37</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>39</v>
@@ -2351,20 +2552,18 @@
         <v>39</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="O12" t="s" s="2">
         <v>118</v>
       </c>
+      <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" t="s" s="2">
         <v>39</v>
@@ -2413,19 +2612,19 @@
         <v>39</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="AH12" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>119</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13">
@@ -2436,11 +2635,11 @@
         <v>120</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" t="s" s="2">
@@ -2456,23 +2655,21 @@
         <v>39</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L13" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="M13" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="N13" t="s" s="2">
         <v>122</v>
       </c>
-      <c r="M13" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>124</v>
-      </c>
       <c r="O13" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="P13" t="s" s="2">
-        <v>125</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="P13" s="2"/>
       <c r="Q13" t="s" s="2">
         <v>39</v>
       </c>
@@ -2508,19 +2705,19 @@
         <v>39</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="AD13" t="s" s="2">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="AE13" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>37</v>
@@ -2532,7 +2729,7 @@
         <v>57</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14">
@@ -2540,10 +2737,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -2569,15 +2766,17 @@
         <v>66</v>
       </c>
       <c r="M14" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="N14" t="s" s="2">
         <v>127</v>
       </c>
-      <c r="N14" t="s" s="2">
+      <c r="O14" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="O14" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="P14" s="2"/>
+      <c r="P14" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="Q14" t="s" s="2">
         <v>39</v>
       </c>
@@ -2586,7 +2785,7 @@
         <v>39</v>
       </c>
       <c r="T14" t="s" s="2">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="U14" t="s" s="2">
         <v>39</v>
@@ -2601,13 +2800,13 @@
         <v>39</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AB14" t="s" s="2">
         <v>39</v>
@@ -2625,10 +2824,10 @@
         <v>39</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>45</v>
@@ -2645,10 +2844,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -2671,18 +2870,20 @@
         <v>46</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="P15" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="P15" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="Q15" t="s" s="2">
         <v>39</v>
       </c>
@@ -2706,13 +2907,13 @@
         <v>39</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="AB15" t="s" s="2">
         <v>39</v>
@@ -2730,7 +2931,7 @@
         <v>39</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>37</v>
@@ -2750,10 +2951,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -2776,18 +2977,20 @@
         <v>46</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="P16" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="P16" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="Q16" t="s" s="2">
         <v>39</v>
       </c>
@@ -2799,7 +3002,7 @@
         <v>39</v>
       </c>
       <c r="U16" t="s" s="2">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="V16" t="s" s="2">
         <v>39</v>
@@ -2811,13 +3014,13 @@
         <v>39</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="AB16" t="s" s="2">
         <v>39</v>
@@ -2835,7 +3038,7 @@
         <v>39</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>37</v>
@@ -2855,10 +3058,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -2869,7 +3072,7 @@
         <v>37</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>39</v>
@@ -2881,16 +3084,16 @@
         <v>46</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" t="s" s="2">
@@ -2904,7 +3107,7 @@
         <v>39</v>
       </c>
       <c r="U17" t="s" s="2">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="V17" t="s" s="2">
         <v>39</v>
@@ -2916,10 +3119,10 @@
         <v>39</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>149</v>
+        <v>39</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>39</v>
@@ -2940,13 +3143,13 @@
         <v>39</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>57</v>
@@ -2960,10 +3163,10 @@
         <v>3</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -2974,7 +3177,7 @@
         <v>37</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I18" t="s" s="2">
         <v>39</v>
@@ -2986,16 +3189,16 @@
         <v>46</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" t="s" s="2">
@@ -3021,10 +3224,10 @@
         <v>39</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>39</v>
@@ -3045,19 +3248,19 @@
         <v>39</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>58</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19">
@@ -3065,10 +3268,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3079,7 +3282,7 @@
         <v>37</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>39</v>
@@ -3091,16 +3294,16 @@
         <v>46</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" t="s" s="2">
@@ -3126,13 +3329,13 @@
         <v>39</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>157</v>
+        <v>39</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="AB19" t="s" s="2">
         <v>39</v>
@@ -3150,19 +3353,19 @@
         <v>39</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>58</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20">
@@ -3170,12 +3373,14 @@
         <v>3</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>178</v>
+      </c>
       <c r="E20" t="s" s="2">
         <v>39</v>
       </c>
@@ -3196,16 +3401,18 @@
         <v>46</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="P20" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="Q20" t="s" s="2">
         <v>39</v>
       </c>
@@ -3253,7 +3460,7 @@
         <v>39</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>37</v>
@@ -3273,10 +3480,10 @@
         <v>3</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3287,7 +3494,7 @@
         <v>37</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>39</v>
@@ -3299,17 +3506,15 @@
         <v>39</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>165</v>
+        <v>117</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="O21" t="s" s="2">
-        <v>167</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" t="s" s="2">
         <v>39</v>
@@ -3358,19 +3563,19 @@
         <v>39</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
@@ -3378,14 +3583,14 @@
         <v>3</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" t="s" s="2">
@@ -3401,19 +3606,19 @@
         <v>39</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>169</v>
+        <v>91</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
@@ -3439,10 +3644,10 @@
         <v>39</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>171</v>
+        <v>39</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>39</v>
@@ -3451,19 +3656,19 @@
         <v>39</v>
       </c>
       <c r="AC22" t="s" s="2">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="AD22" t="s" s="2">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="AE22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>37</v>
@@ -3475,7 +3680,7 @@
         <v>57</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>58</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23">
@@ -3483,10 +3688,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3494,33 +3699,35 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" t="s" s="2">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K23" t="s" s="2">
         <v>46</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>173</v>
+        <v>126</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="P23" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="P23" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="Q23" t="s" s="2">
         <v>39</v>
       </c>
@@ -3529,7 +3736,7 @@
         <v>39</v>
       </c>
       <c r="T23" t="s" s="2">
-        <v>39</v>
+        <v>183</v>
       </c>
       <c r="U23" t="s" s="2">
         <v>39</v>
@@ -3544,13 +3751,13 @@
         <v>39</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="AB23" t="s" s="2">
         <v>39</v>
@@ -3568,13 +3775,13 @@
         <v>39</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>57</v>
@@ -3588,10 +3795,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3611,21 +3818,23 @@
         <v>39</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="P24" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="P24" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="Q24" t="s" s="2">
         <v>39</v>
       </c>
@@ -3649,13 +3858,13 @@
         <v>39</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="Z24" t="s" s="2">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="AB24" t="s" s="2">
         <v>39</v>
@@ -3673,7 +3882,7 @@
         <v>39</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>37</v>
@@ -3693,21 +3902,21 @@
         <v>3</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>183</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" t="s" s="2">
         <v>37</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>39</v>
@@ -3719,18 +3928,20 @@
         <v>46</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="P25" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="P25" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="Q25" t="s" s="2">
         <v>39</v>
       </c>
@@ -3742,7 +3953,7 @@
         <v>39</v>
       </c>
       <c r="U25" t="s" s="2">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="V25" t="s" s="2">
         <v>39</v>
@@ -3778,19 +3989,19 @@
         <v>39</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>119</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26">
@@ -3798,14 +4009,14 @@
         <v>3</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>189</v>
+        <v>39</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" t="s" s="2">
@@ -3824,16 +4035,16 @@
         <v>46</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" t="s" s="2">
@@ -3847,7 +4058,7 @@
         <v>39</v>
       </c>
       <c r="U26" t="s" s="2">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="V26" t="s" s="2">
         <v>39</v>
@@ -3883,7 +4094,7 @@
         <v>39</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>37</v>
@@ -3895,7 +4106,7 @@
         <v>57</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>194</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27">
@@ -3903,10 +4114,10 @@
         <v>3</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -3929,16 +4140,16 @@
         <v>46</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" t="s" s="2">
@@ -3988,7 +4199,7 @@
         <v>39</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>37</v>
@@ -4000,7 +4211,7 @@
         <v>57</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>119</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28">
@@ -4008,10 +4219,10 @@
         <v>3</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4034,16 +4245,16 @@
         <v>46</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="P28" s="2"/>
       <c r="Q28" t="s" s="2">
@@ -4093,7 +4304,7 @@
         <v>39</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>37</v>
@@ -4105,7 +4316,7 @@
         <v>57</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>119</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29">
@@ -4113,10 +4324,10 @@
         <v>3</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4127,7 +4338,7 @@
         <v>37</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>39</v>
@@ -4139,16 +4350,16 @@
         <v>46</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>118</v>
+        <v>192</v>
       </c>
       <c r="P29" s="2"/>
       <c r="Q29" t="s" s="2">
@@ -4198,19 +4409,19 @@
         <v>39</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>119</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30">
@@ -4218,10 +4429,10 @@
         <v>3</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
@@ -4232,7 +4443,7 @@
         <v>37</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>39</v>
@@ -4244,16 +4455,16 @@
         <v>46</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="O30" t="s" s="2">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
@@ -4279,13 +4490,13 @@
         <v>39</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>210</v>
+        <v>39</v>
       </c>
       <c r="AA30" t="s" s="2">
-        <v>211</v>
+        <v>39</v>
       </c>
       <c r="AB30" t="s" s="2">
         <v>39</v>
@@ -4303,19 +4514,19 @@
         <v>39</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>58</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31">
@@ -4323,14 +4534,14 @@
         <v>3</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" t="s" s="2">
@@ -4346,21 +4557,23 @@
         <v>39</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="P31" s="2"/>
+        <v>197</v>
+      </c>
+      <c r="P31" t="s" s="2">
+        <v>203</v>
+      </c>
       <c r="Q31" t="s" s="2">
         <v>39</v>
       </c>
@@ -4408,7 +4621,7 @@
         <v>39</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>37</v>
@@ -4420,7 +4633,7 @@
         <v>57</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>58</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32">
@@ -4428,10 +4641,10 @@
         <v>3</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -4439,30 +4652,32 @@
       </c>
       <c r="F32" s="2"/>
       <c r="G32" t="s" s="2">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>218</v>
+        <v>66</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="O32" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="O32" t="s" s="2">
+        <v>192</v>
+      </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
         <v>39</v>
@@ -4487,13 +4702,13 @@
         <v>39</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>39</v>
+        <v>207</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="AB32" t="s" s="2">
         <v>39</v>
@@ -4511,13 +4726,13 @@
         <v>39</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>57</v>
@@ -4531,10 +4746,10 @@
         <v>3</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -4554,18 +4769,20 @@
         <v>39</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="O33" s="2"/>
+        <v>211</v>
+      </c>
+      <c r="O33" t="s" s="2">
+        <v>212</v>
+      </c>
       <c r="P33" s="2"/>
       <c r="Q33" t="s" s="2">
         <v>39</v>
@@ -4590,13 +4807,13 @@
         <v>39</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>39</v>
+        <v>213</v>
       </c>
       <c r="AA33" t="s" s="2">
-        <v>39</v>
+        <v>214</v>
       </c>
       <c r="AB33" t="s" s="2">
         <v>39</v>
@@ -4614,7 +4831,7 @@
         <v>39</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>37</v>
@@ -4623,10 +4840,10 @@
         <v>45</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34">
@@ -4634,21 +4851,21 @@
         <v>3</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" t="s" s="2">
         <v>37</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>39</v>
@@ -4657,19 +4874,19 @@
         <v>39</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>91</v>
+        <v>216</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="P34" s="2"/>
       <c r="Q34" t="s" s="2">
@@ -4695,43 +4912,43 @@
         <v>39</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="Z34" t="s" s="2">
-        <v>39</v>
+        <v>219</v>
       </c>
       <c r="AA34" t="s" s="2">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="AB34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AC34" t="s" s="2">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="AD34" t="s" s="2">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35">
@@ -4739,14 +4956,14 @@
         <v>3</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>229</v>
+        <v>39</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" t="s" s="2">
@@ -4759,26 +4976,24 @@
         <v>39</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>46</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="O35" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="P35" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
         <v>39</v>
       </c>
@@ -4802,10 +5017,10 @@
         <v>39</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>39</v>
+        <v>224</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>39</v>
@@ -4826,7 +5041,7 @@
         <v>39</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>37</v>
@@ -4838,7 +5053,7 @@
         <v>57</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36">
@@ -4846,10 +5061,10 @@
         <v>3</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -4857,10 +5072,10 @@
       </c>
       <c r="F36" s="2"/>
       <c r="G36" t="s" s="2">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I36" t="s" s="2">
         <v>39</v>
@@ -4869,19 +5084,19 @@
         <v>39</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>113</v>
+        <v>212</v>
       </c>
       <c r="P36" s="2"/>
       <c r="Q36" t="s" s="2">
@@ -4907,10 +5122,10 @@
         <v>39</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="Z36" t="s" s="2">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>39</v>
@@ -4931,13 +5146,13 @@
         <v>39</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>57</v>
@@ -4951,10 +5166,10 @@
         <v>3</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -4965,7 +5180,7 @@
         <v>37</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I37" t="s" s="2">
         <v>39</v>
@@ -4974,19 +5189,19 @@
         <v>39</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>136</v>
+        <v>212</v>
       </c>
       <c r="P37" s="2"/>
       <c r="Q37" t="s" s="2">
@@ -5012,13 +5227,13 @@
         <v>39</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>39</v>
+        <v>232</v>
       </c>
       <c r="AA37" t="s" s="2">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="AB37" t="s" s="2">
         <v>39</v>
@@ -5036,13 +5251,13 @@
         <v>39</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>57</v>
@@ -5056,10 +5271,10 @@
         <v>3</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
@@ -5070,7 +5285,7 @@
         <v>37</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>39</v>
@@ -5079,20 +5294,18 @@
         <v>39</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>110</v>
+        <v>235</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>113</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" t="s" s="2">
         <v>39</v>
@@ -5141,13 +5354,13 @@
         <v>39</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>57</v>
@@ -5161,10 +5374,10 @@
         <v>3</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5187,15 +5400,17 @@
         <v>39</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="O39" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="O39" t="s" s="2">
+        <v>242</v>
+      </c>
       <c r="P39" s="2"/>
       <c r="Q39" t="s" s="2">
         <v>39</v>
@@ -5244,7 +5459,7 @@
         <v>39</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>37</v>
@@ -5264,10 +5479,10 @@
         <v>3</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5278,7 +5493,7 @@
         <v>37</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>39</v>
@@ -5287,18 +5502,20 @@
         <v>39</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="O40" s="2"/>
+        <v>245</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>212</v>
+      </c>
       <c r="P40" s="2"/>
       <c r="Q40" t="s" s="2">
         <v>39</v>
@@ -5323,10 +5540,10 @@
         <v>39</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>39</v>
+        <v>218</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>39</v>
+        <v>246</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>39</v>
@@ -5347,19 +5564,19 @@
         <v>39</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41">
@@ -5367,14 +5584,14 @@
         <v>3</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" t="s" s="2">
@@ -5390,19 +5607,19 @@
         <v>39</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>91</v>
+        <v>248</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="P41" s="2"/>
       <c r="Q41" t="s" s="2">
@@ -5428,31 +5645,31 @@
         <v>39</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>39</v>
+        <v>250</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="AB41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AC41" t="s" s="2">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="AD41" t="s" s="2">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>37</v>
@@ -5464,7 +5681,7 @@
         <v>57</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42">
@@ -5472,46 +5689,44 @@
         <v>3</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
-        <v>229</v>
+        <v>39</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" t="s" s="2">
         <v>37</v>
       </c>
       <c r="H42" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
         <v>39</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>90</v>
+        <v>253</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="P42" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="P42" s="2"/>
       <c r="Q42" t="s" s="2">
         <v>39</v>
       </c>
@@ -5559,19 +5774,19 @@
         <v>39</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43">
@@ -5579,21 +5794,21 @@
         <v>3</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>39</v>
+        <v>258</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" t="s" s="2">
         <v>37</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I43" t="s" s="2">
         <v>39</v>
@@ -5602,19 +5817,19 @@
         <v>39</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>110</v>
+        <v>259</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>113</v>
+        <v>262</v>
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" t="s" s="2">
@@ -5664,19 +5879,19 @@
         <v>39</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>57</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>58</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44">
@@ -5684,14 +5899,14 @@
         <v>3</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>39</v>
+        <v>264</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" t="s" s="2">
@@ -5707,19 +5922,19 @@
         <v>39</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" t="s" s="2">
@@ -5745,13 +5960,13 @@
         <v>39</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>254</v>
+        <v>39</v>
       </c>
       <c r="AA44" t="s" s="2">
-        <v>255</v>
+        <v>39</v>
       </c>
       <c r="AB44" t="s" s="2">
         <v>39</v>
@@ -5769,7 +5984,7 @@
         <v>39</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>37</v>
@@ -5781,6 +5996,1892 @@
         <v>57</v>
       </c>
       <c r="AK44" t="s" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="O45" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="P45" s="2"/>
+      <c r="Q45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R45" s="2"/>
+      <c r="S45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="O46" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="P46" s="2"/>
+      <c r="Q46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R46" s="2"/>
+      <c r="S46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="O47" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R47" s="2"/>
+      <c r="S47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="O48" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="P48" s="2"/>
+      <c r="Q48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R48" s="2"/>
+      <c r="S48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="O49" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="P49" s="2"/>
+      <c r="Q49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R49" s="2"/>
+      <c r="S49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R50" s="2"/>
+      <c r="S50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R51" s="2"/>
+      <c r="S51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R52" s="2"/>
+      <c r="S52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="P53" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="Q53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R53" s="2"/>
+      <c r="S53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R54" s="2"/>
+      <c r="S54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="C55" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R55" s="2"/>
+      <c r="S55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="O56" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R56" s="2"/>
+      <c r="S56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R57" s="2"/>
+      <c r="S57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H58" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R58" s="2"/>
+      <c r="S58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG58" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="AH58" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI58" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="O59" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="P59" s="2"/>
+      <c r="Q59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R59" s="2"/>
+      <c r="S59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AE59" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF59" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="AH59" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI59" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="C60" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="I60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J60" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="O60" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="P60" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="Q60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R60" s="2"/>
+      <c r="S60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="C61" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="O61" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R61" s="2"/>
+      <c r="S61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="C62" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="O62" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R62" s="2"/>
+      <c r="S62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="AK62" t="s" s="2">
         <v>58</v>
       </c>
     </row>

</xml_diff>